<commit_message>
Uusi tehtävälista on syntynyt.
</commit_message>
<xml_diff>
--- a/documents/Tehtävälista ja julkaisukäyrä, Java, Sprintti 2.xlsx
+++ b/documents/Tehtävälista ja julkaisukäyrä, Java, Sprintti 2.xlsx
@@ -92,9 +92,6 @@
     <t>Jonkin asian selvittäminen (miten tehdään tms.)</t>
   </si>
   <si>
-    <t>Sprintti 1</t>
-  </si>
-  <si>
     <t>Random tehtäviä</t>
   </si>
   <si>
@@ -198,6 +195,9 @@
   </si>
   <si>
     <t>HP</t>
+  </si>
+  <si>
+    <t>Sprintti 3</t>
   </si>
 </sst>
 </file>
@@ -678,22 +678,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>84</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>68</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>52</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>36</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>20</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -748,10 +748,10 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>84</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>68</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -777,11 +777,11 @@
         </c:hiLowLines>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="142289536"/>
-        <c:axId val="142320384"/>
+        <c:axId val="97609984"/>
+        <c:axId val="97624448"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="142289536"/>
+        <c:axId val="97609984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -810,7 +810,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="142320384"/>
+        <c:crossAx val="97624448"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -818,7 +818,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="142320384"/>
+        <c:axId val="97624448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -848,7 +848,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="142289536"/>
+        <c:crossAx val="97609984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1587,7 +1587,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E22" sqref="E22"/>
+      <selection pane="bottomRight" activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1631,7 +1631,7 @@
         <v>8</v>
       </c>
       <c r="I1" s="42" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J1" s="30"/>
       <c r="K1" s="30"/>
@@ -1650,11 +1650,11 @@
         <v>1</v>
       </c>
       <c r="B2" s="33" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C2" s="33"/>
       <c r="D2" s="33" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E2" s="33">
         <v>16</v>
@@ -1668,7 +1668,7 @@
       <c r="H2" s="34"/>
       <c r="I2" s="43">
         <f>'Sprintti 2'!C8</f>
-        <v>80</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1676,10 +1676,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="35" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D3" s="35" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E3" s="35">
         <v>3</v>
@@ -1692,7 +1692,7 @@
       </c>
       <c r="H3" s="34"/>
       <c r="I3" s="44" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:20" ht="15" x14ac:dyDescent="0.25">
@@ -1700,13 +1700,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="35" t="s">
+        <v>46</v>
+      </c>
+      <c r="C4" s="35" t="s">
         <v>47</v>
       </c>
-      <c r="C4" s="35" t="s">
-        <v>48</v>
-      </c>
       <c r="D4" s="35" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E4" s="35">
         <v>2</v>
@@ -1719,7 +1719,7 @@
       </c>
       <c r="H4" s="34"/>
       <c r="I4" s="44" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1727,10 +1727,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="35" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D5" s="35" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E5" s="35">
         <v>3</v>
@@ -1742,7 +1742,7 @@
         <v>10</v>
       </c>
       <c r="I5" s="44" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1750,13 +1750,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="35" t="s">
+        <v>49</v>
+      </c>
+      <c r="C6" s="35" t="s">
         <v>50</v>
       </c>
-      <c r="C6" s="35" t="s">
+      <c r="D6" s="35" t="s">
         <v>51</v>
-      </c>
-      <c r="D6" s="35" t="s">
-        <v>52</v>
       </c>
       <c r="E6" s="35">
         <v>3</v>
@@ -1774,10 +1774,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="35" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D7" s="35" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E7" s="35">
         <v>4</v>
@@ -1798,10 +1798,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="35" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D8" s="35" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E8" s="35">
         <v>4</v>
@@ -1818,13 +1818,13 @@
         <v>8</v>
       </c>
       <c r="B9" s="35" t="s">
+        <v>40</v>
+      </c>
+      <c r="C9" s="35" t="s">
         <v>41</v>
       </c>
-      <c r="C9" s="35" t="s">
+      <c r="D9" s="35" t="s">
         <v>42</v>
-      </c>
-      <c r="D9" s="35" t="s">
-        <v>43</v>
       </c>
       <c r="E9" s="35">
         <v>6</v>
@@ -1844,10 +1844,10 @@
         <v>24</v>
       </c>
       <c r="C10" s="37" t="s">
+        <v>43</v>
+      </c>
+      <c r="D10" s="38" t="s">
         <v>44</v>
-      </c>
-      <c r="D10" s="38" t="s">
-        <v>45</v>
       </c>
       <c r="E10" s="36">
         <v>15</v>
@@ -1864,11 +1864,11 @@
         <v>10</v>
       </c>
       <c r="B11" s="36" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C11" s="37"/>
       <c r="D11" s="38" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E11" s="36">
         <v>4</v>
@@ -1877,7 +1877,7 @@
         <v>2</v>
       </c>
       <c r="G11" s="39" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="12" spans="1:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1885,10 +1885,10 @@
         <v>11</v>
       </c>
       <c r="B12" s="38" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D12" s="38" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E12" s="38">
         <v>4</v>
@@ -1905,10 +1905,10 @@
         <v>12</v>
       </c>
       <c r="B13" s="38" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D13" s="38" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E13" s="38">
         <v>6</v>
@@ -1925,10 +1925,10 @@
         <v>13</v>
       </c>
       <c r="B14" s="38" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D14" s="38" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E14" s="38">
         <v>10</v>
@@ -1942,19 +1942,19 @@
     </row>
     <row r="15" spans="1:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="46" t="s">
+        <v>56</v>
+      </c>
+      <c r="D15" s="35" t="s">
+        <v>42</v>
+      </c>
+      <c r="E15" s="35" t="s">
         <v>57</v>
-      </c>
-      <c r="D15" s="35" t="s">
-        <v>43</v>
-      </c>
-      <c r="E15" s="35" t="s">
-        <v>58</v>
       </c>
       <c r="F15" s="35">
         <v>1</v>
       </c>
       <c r="G15" s="41" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="16" spans="1:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1962,16 +1962,19 @@
         <v>14</v>
       </c>
       <c r="B16" s="35" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D16" s="35" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E16" s="35">
         <v>4</v>
       </c>
+      <c r="F16" s="35">
+        <v>1</v>
+      </c>
       <c r="G16" s="41" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="22" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2090,7 +2093,7 @@
   <dimension ref="A1:S42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M4" sqref="M4"/>
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2117,7 +2120,7 @@
     <row r="1" spans="1:19" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2"/>
       <c r="B1" s="3" t="s">
-        <v>25</v>
+        <v>60</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="4"/>
@@ -2139,22 +2142,22 @@
         <v>21</v>
       </c>
       <c r="N1" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="O1" s="23" t="s">
         <v>53</v>
       </c>
-      <c r="O1" s="23" t="s">
+      <c r="P1" s="23" t="s">
         <v>54</v>
       </c>
-      <c r="P1" s="23" t="s">
+      <c r="Q1" s="23" t="s">
         <v>55</v>
       </c>
-      <c r="Q1" s="23" t="s">
-        <v>56</v>
-      </c>
       <c r="R1" s="23" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="S1" s="23" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2163,7 +2166,7 @@
         <v>12</v>
       </c>
       <c r="C2" s="25">
-        <v>41367</v>
+        <v>41394</v>
       </c>
       <c r="D2" s="7"/>
       <c r="I2" s="2"/>
@@ -2172,12 +2175,10 @@
         <v>0</v>
       </c>
       <c r="L2" s="17">
-        <f>SUM('Sprintin tehtävälista'!E2:E100)</f>
-        <v>84</v>
+        <v>20</v>
       </c>
       <c r="M2" s="17">
-        <f>L2</f>
-        <v>84</v>
+        <v>20</v>
       </c>
       <c r="N2" s="17"/>
       <c r="O2" s="17"/>
@@ -2192,23 +2193,21 @@
         <v>13</v>
       </c>
       <c r="C3" s="25">
-        <v>41381</v>
+        <v>41424</v>
       </c>
       <c r="D3" s="7"/>
       <c r="I3" s="2"/>
       <c r="J3" s="25">
-        <v>41367</v>
+        <v>41394</v>
       </c>
       <c r="K3" s="24">
         <v>1</v>
       </c>
       <c r="L3" s="24">
-        <f>L2-($C$5*$C$7)</f>
-        <v>68</v>
+        <v>16</v>
       </c>
       <c r="M3" s="16">
-        <f>M2-SUM(N3:U3)</f>
-        <v>68</v>
+        <v>16</v>
       </c>
       <c r="N3" s="21">
         <v>4</v>
@@ -2237,14 +2236,13 @@
       <c r="D4" s="7"/>
       <c r="I4" s="2"/>
       <c r="J4" s="25">
-        <v>41373</v>
+        <v>41401</v>
       </c>
       <c r="K4" s="24">
         <v>2</v>
       </c>
       <c r="L4" s="24">
-        <f t="shared" ref="L4:L7" si="0">L3-($C$5*$C$7)</f>
-        <v>52</v>
+        <v>12</v>
       </c>
       <c r="M4" s="20"/>
       <c r="N4" s="22">
@@ -2273,14 +2271,13 @@
       <c r="D5" s="7"/>
       <c r="I5" s="2"/>
       <c r="J5" s="25">
-        <v>41374</v>
+        <v>41408</v>
       </c>
       <c r="K5" s="24">
         <v>3</v>
       </c>
       <c r="L5" s="24">
-        <f t="shared" si="0"/>
-        <v>36</v>
+        <v>8</v>
       </c>
       <c r="M5" s="20"/>
       <c r="N5" s="22">
@@ -2309,14 +2306,13 @@
       <c r="D6" s="7"/>
       <c r="I6" s="2"/>
       <c r="J6" s="25">
-        <v>41380</v>
+        <v>41415</v>
       </c>
       <c r="K6" s="24">
         <v>4</v>
       </c>
       <c r="L6" s="24">
-        <f t="shared" si="0"/>
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="M6" s="20"/>
       <c r="N6" s="22">
@@ -2345,14 +2341,13 @@
       <c r="D7" s="7"/>
       <c r="I7" s="2"/>
       <c r="J7" s="25">
-        <v>41381</v>
+        <v>41422</v>
       </c>
       <c r="K7" s="24">
         <v>5</v>
       </c>
       <c r="L7" s="24">
-        <f t="shared" si="0"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="M7" s="20"/>
       <c r="N7" s="22">
@@ -2376,8 +2371,7 @@
         <v>16</v>
       </c>
       <c r="C8" s="16">
-        <f>C5*C6*C7</f>
-        <v>80</v>
+        <v>20</v>
       </c>
       <c r="D8" s="7"/>
     </row>
@@ -2638,21 +2632,21 @@
       </c>
     </row>
     <row r="21" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="17" t="e">
-        <f>'Sprintin tehtävälista'!#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="B21" s="17" t="e">
-        <f>'Sprintin tehtävälista'!#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="C21" s="18" t="e">
-        <f>'Sprintin tehtävälista'!#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D21" s="19" t="e">
-        <f>'Sprintin tehtävälista'!#REF!</f>
-        <v>#REF!</v>
+      <c r="A21" s="17" t="str">
+        <f>'Sprintin tehtävälista'!D15</f>
+        <v>Sami K</v>
+      </c>
+      <c r="B21" s="17" t="str">
+        <f>'Sprintin tehtävälista'!B15</f>
+        <v>Mein Kampf</v>
+      </c>
+      <c r="C21" s="18" t="str">
+        <f>'Sprintin tehtävälista'!E15</f>
+        <v>SS</v>
+      </c>
+      <c r="D21" s="19" t="str">
+        <f>'Sprintin tehtävälista'!G15</f>
+        <v>Valmis</v>
       </c>
       <c r="E21" s="7"/>
       <c r="F21" s="1" t="e">
@@ -2669,21 +2663,21 @@
       </c>
     </row>
     <row r="22" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="17" t="e">
-        <f>'Sprintin tehtävälista'!#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="B22" s="17" t="e">
-        <f>'Sprintin tehtävälista'!#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="C22" s="18" t="e">
-        <f>'Sprintin tehtävälista'!#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D22" s="19" t="e">
-        <f>'Sprintin tehtävälista'!#REF!</f>
-        <v>#REF!</v>
+      <c r="A22" s="17" t="str">
+        <f>'Sprintin tehtävälista'!D16</f>
+        <v>Sami K</v>
+      </c>
+      <c r="B22" s="17" t="str">
+        <f>'Sprintin tehtävälista'!B16</f>
+        <v>HP</v>
+      </c>
+      <c r="C22" s="18">
+        <f>'Sprintin tehtävälista'!E16</f>
+        <v>4</v>
+      </c>
+      <c r="D22" s="19" t="str">
+        <f>'Sprintin tehtävälista'!G16</f>
+        <v>Valmis</v>
       </c>
       <c r="E22" s="7"/>
       <c r="F22" s="1" t="e">
@@ -2700,21 +2694,21 @@
       </c>
     </row>
     <row r="23" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="17" t="e">
-        <f>'Sprintin tehtävälista'!#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="B23" s="17" t="e">
-        <f>'Sprintin tehtävälista'!#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="C23" s="18" t="e">
-        <f>'Sprintin tehtävälista'!#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D23" s="19" t="e">
-        <f>'Sprintin tehtävälista'!#REF!</f>
-        <v>#REF!</v>
+      <c r="A23" s="17">
+        <f>'Sprintin tehtävälista'!D17</f>
+        <v>0</v>
+      </c>
+      <c r="B23" s="17">
+        <f>'Sprintin tehtävälista'!B17</f>
+        <v>0</v>
+      </c>
+      <c r="C23" s="18">
+        <f>'Sprintin tehtävälista'!E17</f>
+        <v>0</v>
+      </c>
+      <c r="D23" s="19">
+        <f>'Sprintin tehtävälista'!G17</f>
+        <v>0</v>
       </c>
       <c r="E23" s="7"/>
       <c r="F23" s="1" t="e">
@@ -2731,21 +2725,21 @@
       </c>
     </row>
     <row r="24" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="17" t="e">
-        <f>'Sprintin tehtävälista'!#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="B24" s="17" t="e">
-        <f>'Sprintin tehtävälista'!#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="C24" s="18" t="e">
-        <f>'Sprintin tehtävälista'!#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D24" s="19" t="e">
-        <f>'Sprintin tehtävälista'!#REF!</f>
-        <v>#REF!</v>
+      <c r="A24" s="17">
+        <f>'Sprintin tehtävälista'!D18</f>
+        <v>0</v>
+      </c>
+      <c r="B24" s="17">
+        <f>'Sprintin tehtävälista'!B18</f>
+        <v>0</v>
+      </c>
+      <c r="C24" s="18">
+        <f>'Sprintin tehtävälista'!E18</f>
+        <v>0</v>
+      </c>
+      <c r="D24" s="19">
+        <f>'Sprintin tehtävälista'!G18</f>
+        <v>0</v>
       </c>
       <c r="E24" s="7"/>
       <c r="F24" s="1" t="e">
@@ -2762,21 +2756,21 @@
       </c>
     </row>
     <row r="25" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="17" t="e">
-        <f>'Sprintin tehtävälista'!#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="B25" s="17" t="e">
-        <f>'Sprintin tehtävälista'!#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="C25" s="18" t="e">
-        <f>'Sprintin tehtävälista'!#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D25" s="19" t="e">
-        <f>'Sprintin tehtävälista'!#REF!</f>
-        <v>#REF!</v>
+      <c r="A25" s="17">
+        <f>'Sprintin tehtävälista'!D19</f>
+        <v>0</v>
+      </c>
+      <c r="B25" s="17">
+        <f>'Sprintin tehtävälista'!B19</f>
+        <v>0</v>
+      </c>
+      <c r="C25" s="18">
+        <f>'Sprintin tehtävälista'!E19</f>
+        <v>0</v>
+      </c>
+      <c r="D25" s="19">
+        <f>'Sprintin tehtävälista'!G19</f>
+        <v>0</v>
       </c>
       <c r="E25" s="7"/>
       <c r="F25" s="1" t="e">
@@ -2793,21 +2787,21 @@
       </c>
     </row>
     <row r="26" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="17" t="e">
-        <f>'Sprintin tehtävälista'!#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="B26" s="17" t="e">
-        <f>'Sprintin tehtävälista'!#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="C26" s="18" t="e">
-        <f>'Sprintin tehtävälista'!#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D26" s="19" t="e">
-        <f>'Sprintin tehtävälista'!#REF!</f>
-        <v>#REF!</v>
+      <c r="A26" s="17">
+        <f>'Sprintin tehtävälista'!D20</f>
+        <v>0</v>
+      </c>
+      <c r="B26" s="17">
+        <f>'Sprintin tehtävälista'!B20</f>
+        <v>0</v>
+      </c>
+      <c r="C26" s="18">
+        <f>'Sprintin tehtävälista'!E20</f>
+        <v>0</v>
+      </c>
+      <c r="D26" s="19">
+        <f>'Sprintin tehtävälista'!G20</f>
+        <v>0</v>
       </c>
       <c r="E26" s="7"/>
       <c r="F26" s="1" t="e">
@@ -2824,232 +2818,232 @@
       </c>
     </row>
     <row r="27" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="17" t="e">
-        <f>'Sprintin tehtävälista'!#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="B27" s="17" t="e">
-        <f>'Sprintin tehtävälista'!#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="C27" s="18" t="e">
-        <f>'Sprintin tehtävälista'!#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D27" s="19" t="e">
-        <f>'Sprintin tehtävälista'!#REF!</f>
-        <v>#REF!</v>
+      <c r="A27" s="17">
+        <f>'Sprintin tehtävälista'!D21</f>
+        <v>0</v>
+      </c>
+      <c r="B27" s="17">
+        <f>'Sprintin tehtävälista'!B21</f>
+        <v>0</v>
+      </c>
+      <c r="C27" s="18">
+        <f>'Sprintin tehtävälista'!E21</f>
+        <v>0</v>
+      </c>
+      <c r="D27" s="19">
+        <f>'Sprintin tehtävälista'!G21</f>
+        <v>0</v>
       </c>
       <c r="E27" s="7"/>
       <c r="F27" s="1" t="e">
         <f>VLOOKUP(A21, 'Sprintin tehtävälista'!$A$2:$E$84, 5, FALSE)</f>
-        <v>#REF!</v>
+        <v>#N/A</v>
       </c>
       <c r="G27" s="10" t="e">
         <f>VLOOKUP(A21, 'Sprintin tehtävälista'!$A$2:$B$84, 2, FALSE)</f>
-        <v>#REF!</v>
+        <v>#N/A</v>
       </c>
       <c r="H27" s="13" t="e">
         <f>VLOOKUP(A21, 'Sprintin tehtävälista'!$A$2:$G$84, 7, FALSE)</f>
-        <v>#REF!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="17" t="e">
-        <f>'Sprintin tehtävälista'!#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="B28" s="17" t="e">
-        <f>'Sprintin tehtävälista'!#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="C28" s="18" t="e">
-        <f>'Sprintin tehtävälista'!#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D28" s="19" t="e">
-        <f>'Sprintin tehtävälista'!#REF!</f>
-        <v>#REF!</v>
+      <c r="A28" s="17">
+        <f>'Sprintin tehtävälista'!D22</f>
+        <v>0</v>
+      </c>
+      <c r="B28" s="17">
+        <f>'Sprintin tehtävälista'!B22</f>
+        <v>0</v>
+      </c>
+      <c r="C28" s="18">
+        <f>'Sprintin tehtävälista'!E22</f>
+        <v>0</v>
+      </c>
+      <c r="D28" s="19">
+        <f>'Sprintin tehtävälista'!G22</f>
+        <v>0</v>
       </c>
       <c r="E28" s="7"/>
       <c r="F28" s="1" t="e">
         <f>VLOOKUP(A22, 'Sprintin tehtävälista'!$A$2:$E$84, 5, FALSE)</f>
-        <v>#REF!</v>
+        <v>#N/A</v>
       </c>
       <c r="G28" s="10" t="e">
         <f>VLOOKUP(A22, 'Sprintin tehtävälista'!$A$2:$B$84, 2, FALSE)</f>
-        <v>#REF!</v>
+        <v>#N/A</v>
       </c>
       <c r="H28" s="13" t="e">
         <f>VLOOKUP(A22, 'Sprintin tehtävälista'!$A$2:$G$84, 7, FALSE)</f>
-        <v>#REF!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="17" t="e">
-        <f>'Sprintin tehtävälista'!#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="B29" s="17" t="e">
-        <f>'Sprintin tehtävälista'!#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="C29" s="18" t="e">
-        <f>'Sprintin tehtävälista'!#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D29" s="19" t="e">
-        <f>'Sprintin tehtävälista'!#REF!</f>
-        <v>#REF!</v>
+      <c r="A29" s="17">
+        <f>'Sprintin tehtävälista'!D23</f>
+        <v>0</v>
+      </c>
+      <c r="B29" s="17">
+        <f>'Sprintin tehtävälista'!B23</f>
+        <v>0</v>
+      </c>
+      <c r="C29" s="18">
+        <f>'Sprintin tehtävälista'!E23</f>
+        <v>0</v>
+      </c>
+      <c r="D29" s="19">
+        <f>'Sprintin tehtävälista'!G23</f>
+        <v>0</v>
       </c>
       <c r="E29" s="7"/>
       <c r="F29" s="1" t="e">
         <f>VLOOKUP(A23, 'Sprintin tehtävälista'!$A$2:$E$84, 5, FALSE)</f>
-        <v>#REF!</v>
+        <v>#N/A</v>
       </c>
       <c r="G29" s="10" t="e">
         <f>VLOOKUP(A23, 'Sprintin tehtävälista'!$A$2:$B$84, 2, FALSE)</f>
-        <v>#REF!</v>
+        <v>#N/A</v>
       </c>
       <c r="H29" s="13" t="e">
         <f>VLOOKUP(A23, 'Sprintin tehtävälista'!$A$2:$G$84, 7, FALSE)</f>
-        <v>#REF!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="17" t="e">
-        <f>'Sprintin tehtävälista'!#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="B30" s="17" t="e">
-        <f>'Sprintin tehtävälista'!#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="C30" s="18" t="e">
-        <f>'Sprintin tehtävälista'!#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D30" s="19" t="e">
-        <f>'Sprintin tehtävälista'!#REF!</f>
-        <v>#REF!</v>
+      <c r="A30" s="17">
+        <f>'Sprintin tehtävälista'!D24</f>
+        <v>0</v>
+      </c>
+      <c r="B30" s="17">
+        <f>'Sprintin tehtävälista'!B24</f>
+        <v>0</v>
+      </c>
+      <c r="C30" s="18">
+        <f>'Sprintin tehtävälista'!E24</f>
+        <v>0</v>
+      </c>
+      <c r="D30" s="19">
+        <f>'Sprintin tehtävälista'!G24</f>
+        <v>0</v>
       </c>
       <c r="E30" s="7"/>
       <c r="F30" s="1" t="e">
         <f>VLOOKUP(A24, 'Sprintin tehtävälista'!$A$2:$E$84, 5, FALSE)</f>
-        <v>#REF!</v>
+        <v>#N/A</v>
       </c>
       <c r="G30" s="10" t="e">
         <f>VLOOKUP(A24, 'Sprintin tehtävälista'!$A$2:$B$84, 2, FALSE)</f>
-        <v>#REF!</v>
+        <v>#N/A</v>
       </c>
       <c r="H30" s="13" t="e">
         <f>VLOOKUP(A24, 'Sprintin tehtävälista'!$A$2:$G$84, 7, FALSE)</f>
-        <v>#REF!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="17">
-        <f>'Sprintin tehtävälista'!D22</f>
+        <f>'Sprintin tehtävälista'!D25</f>
         <v>0</v>
       </c>
       <c r="B31" s="17">
-        <f>'Sprintin tehtävälista'!B22</f>
+        <f>'Sprintin tehtävälista'!B25</f>
         <v>0</v>
       </c>
       <c r="C31" s="18">
-        <f>'Sprintin tehtävälista'!E22</f>
+        <f>'Sprintin tehtävälista'!E25</f>
         <v>0</v>
       </c>
       <c r="D31" s="19">
-        <f>'Sprintin tehtävälista'!G22</f>
+        <f>'Sprintin tehtävälista'!G25</f>
         <v>0</v>
       </c>
       <c r="E31" s="7"/>
       <c r="F31" s="1" t="e">
         <f>VLOOKUP(A25, 'Sprintin tehtävälista'!$A$2:$E$84, 5, FALSE)</f>
-        <v>#REF!</v>
+        <v>#N/A</v>
       </c>
       <c r="G31" s="10" t="e">
         <f>VLOOKUP(A25, 'Sprintin tehtävälista'!$A$2:$B$84, 2, FALSE)</f>
-        <v>#REF!</v>
+        <v>#N/A</v>
       </c>
       <c r="H31" s="13" t="e">
         <f>VLOOKUP(A25, 'Sprintin tehtävälista'!$A$2:$G$84, 7, FALSE)</f>
-        <v>#REF!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E32" s="7"/>
       <c r="F32" s="1" t="e">
         <f>VLOOKUP(A26, 'Sprintin tehtävälista'!$A$2:$E$84, 5, FALSE)</f>
-        <v>#REF!</v>
+        <v>#N/A</v>
       </c>
       <c r="G32" s="10" t="e">
         <f>VLOOKUP(A26, 'Sprintin tehtävälista'!$A$2:$B$84, 2, FALSE)</f>
-        <v>#REF!</v>
+        <v>#N/A</v>
       </c>
       <c r="H32" s="13" t="e">
         <f>VLOOKUP(A26, 'Sprintin tehtävälista'!$A$2:$G$84, 7, FALSE)</f>
-        <v>#REF!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="33" spans="5:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E33" s="7"/>
       <c r="F33" s="1" t="e">
         <f>VLOOKUP(A27, 'Sprintin tehtävälista'!$A$2:$E$84, 5, FALSE)</f>
-        <v>#REF!</v>
+        <v>#N/A</v>
       </c>
       <c r="G33" s="10" t="e">
         <f>VLOOKUP(A27, 'Sprintin tehtävälista'!$A$2:$B$84, 2, FALSE)</f>
-        <v>#REF!</v>
+        <v>#N/A</v>
       </c>
       <c r="H33" s="13" t="e">
         <f>VLOOKUP(A27, 'Sprintin tehtävälista'!$A$2:$G$84, 7, FALSE)</f>
-        <v>#REF!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="34" spans="5:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E34" s="7"/>
       <c r="F34" s="1" t="e">
         <f>VLOOKUP(A28, 'Sprintin tehtävälista'!$A$2:$E$84, 5, FALSE)</f>
-        <v>#REF!</v>
+        <v>#N/A</v>
       </c>
       <c r="G34" s="10" t="e">
         <f>VLOOKUP(A28, 'Sprintin tehtävälista'!$A$2:$B$84, 2, FALSE)</f>
-        <v>#REF!</v>
+        <v>#N/A</v>
       </c>
       <c r="H34" s="13" t="e">
         <f>VLOOKUP(A28, 'Sprintin tehtävälista'!$A$2:$G$84, 7, FALSE)</f>
-        <v>#REF!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="35" spans="5:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E35" s="7"/>
       <c r="F35" s="1" t="e">
         <f>VLOOKUP(A29, 'Sprintin tehtävälista'!$A$2:$E$84, 5, FALSE)</f>
-        <v>#REF!</v>
+        <v>#N/A</v>
       </c>
       <c r="G35" s="10" t="e">
         <f>VLOOKUP(A29, 'Sprintin tehtävälista'!$A$2:$B$84, 2, FALSE)</f>
-        <v>#REF!</v>
+        <v>#N/A</v>
       </c>
       <c r="H35" s="13" t="e">
         <f>VLOOKUP(A29, 'Sprintin tehtävälista'!$A$2:$G$84, 7, FALSE)</f>
-        <v>#REF!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="36" spans="5:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F36" t="e">
         <f>VLOOKUP(A30, 'Sprintin tehtävälista'!$A$2:$E$84, 5, FALSE)</f>
-        <v>#REF!</v>
+        <v>#N/A</v>
       </c>
       <c r="G36" t="e">
         <f>VLOOKUP(A30, 'Sprintin tehtävälista'!$A$2:$B$84, 2, FALSE)</f>
-        <v>#REF!</v>
+        <v>#N/A</v>
       </c>
       <c r="H36" t="e">
         <f>VLOOKUP(A30, 'Sprintin tehtävälista'!$A$2:$G$84, 7, FALSE)</f>
-        <v>#REF!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="37" spans="5:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3082,7 +3076,7 @@
       <c r="H42"/>
     </row>
   </sheetData>
-  <sheetProtection password="CAE1" sheet="1" objects="1" scenarios="1" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0" selectLockedCells="1"/>
+  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0" selectLockedCells="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>

</xml_diff>